<commit_message>
add new shop table
</commit_message>
<xml_diff>
--- a/ReadMeMore.xlsx
+++ b/ReadMeMore.xlsx
@@ -589,7 +589,8 @@
 2:INVENTORY_TRANSACTION_HIST_TAB
 3:N_AIS_SHOP_LIST_PICKED_ACT_TAB
 4:N_TRANSPORT_ORDER_TAB
-5:SHOP_ORD_TAB,SHOP_ORDER_OPERATION_TAB</t>
+5:SHOP_ORD_TAB,SHOP_ORDER_OPERATION_TAB
+6:SHOP_ORD_TAB,SHOP_MATERIAL_ALLOC_TAB</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1656,8 +1657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:L9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1772,7 +1773,7 @@
       <c r="K9" s="11"/>
       <c r="L9" s="11"/>
     </row>
-    <row r="10" spans="1:14" ht="87.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:14" ht="98.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="11" t="s">
         <v>66</v>
       </c>

</xml_diff>